<commit_message>
epic spread sheet update
</commit_message>
<xml_diff>
--- a/epic-spread-sheet.xlsx
+++ b/epic-spread-sheet.xlsx
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,14 +1229,14 @@
         <v>32</v>
       </c>
       <c r="H4" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I4" s="3">
         <f>(H4+J4-50)*I27</f>
-        <v>2600</v>
+        <v>1600</v>
       </c>
       <c r="J4" s="3">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>20</v>
@@ -1291,10 +1291,10 @@
       </c>
       <c r="I5" s="3">
         <f>(H5+J5-50)*I27</f>
-        <v>4800</v>
+        <v>2800</v>
       </c>
       <c r="J5" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>23</v>

</xml_diff>